<commit_message>
First pass at translating to python3
</commit_message>
<xml_diff>
--- a/RemoteYearBot/SampleData_RealAnon2020/forBot_FacultyAvailabilityMatrix.xlsx
+++ b/RemoteYearBot/SampleData_RealAnon2020/forBot_FacultyAvailabilityMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/RemoteYearBot/SampleData_RealAnon2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C1FD99-929B-D944-99E2-4498D3643FE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C9C779-2184-2A48-BFA5-9C12C80980C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20100" yWindow="580" windowWidth="45560" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28020" yWindow="460" windowWidth="39720" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="169">
   <si>
     <t>Scott Atwood</t>
   </si>
@@ -542,6 +542,9 @@
   </si>
   <si>
     <t>Zoom room: 123456833</t>
+  </si>
+  <si>
+    <t>Contact</t>
   </si>
 </sst>
 </file>
@@ -1095,11 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW35"/>
+  <dimension ref="A1:AU35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H10" sqref="H10"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1148,7 @@
     <col min="47" max="47" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="23" t="s">
         <v>28</v>
       </c>
@@ -1284,10 +1287,11 @@
       <c r="AU1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-    </row>
-    <row r="2" spans="1:49" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:47" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>168</v>
+      </c>
       <c r="B2" s="27" t="s">
         <v>123</v>
       </c>
@@ -1426,10 +1430,8 @@
       <c r="AU2" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="AV2" s="18"/>
-      <c r="AW2" s="18"/>
-    </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>43</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>91</v>
       </c>
@@ -1590,10 +1592,8 @@
       <c r="AU4" s="3">
         <v>1</v>
       </c>
-      <c r="AV4" s="18"/>
-      <c r="AW4" s="18"/>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>92</v>
       </c>
@@ -1679,10 +1679,8 @@
       <c r="AU5" s="2">
         <v>1</v>
       </c>
-      <c r="AV5" s="18"/>
-      <c r="AW5" s="18"/>
-    </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>93</v>
       </c>
@@ -1776,10 +1774,8 @@
       <c r="AU6" s="2">
         <v>1</v>
       </c>
-      <c r="AV6" s="18"/>
-      <c r="AW6" s="18"/>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
@@ -1867,10 +1863,8 @@
       <c r="AU7" s="2">
         <v>1</v>
       </c>
-      <c r="AV7" s="18"/>
-      <c r="AW7" s="18"/>
-    </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>95</v>
       </c>
@@ -1937,7 +1931,9 @@
         <v>1</v>
       </c>
       <c r="AP8" s="2"/>
-      <c r="AQ8" s="2"/>
+      <c r="AQ8" s="2">
+        <v>1</v>
+      </c>
       <c r="AR8" s="12">
         <v>1</v>
       </c>
@@ -1948,10 +1944,8 @@
       <c r="AU8" s="2">
         <v>1</v>
       </c>
-      <c r="AV8" s="18"/>
-      <c r="AW8" s="18"/>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>96</v>
       </c>
@@ -2023,10 +2017,8 @@
       <c r="AU9" s="11">
         <v>1</v>
       </c>
-      <c r="AV9" s="18"/>
-      <c r="AW9" s="18"/>
-    </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>97</v>
       </c>
@@ -2122,10 +2114,8 @@
       <c r="AU10" s="2">
         <v>1</v>
       </c>
-      <c r="AV10" s="18"/>
-      <c r="AW10" s="18"/>
-    </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>98</v>
       </c>
@@ -2221,10 +2211,8 @@
       <c r="AU11" s="2">
         <v>1</v>
       </c>
-      <c r="AV11" s="18"/>
-      <c r="AW11" s="18"/>
-    </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>107</v>
       </c>
@@ -2320,10 +2308,8 @@
       <c r="AU12" s="2">
         <v>1</v>
       </c>
-      <c r="AV12" s="18"/>
-      <c r="AW12" s="18"/>
-    </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
@@ -2419,10 +2405,8 @@
       <c r="AU13" s="2">
         <v>1</v>
       </c>
-      <c r="AV13" s="18"/>
-      <c r="AW13" s="18"/>
-    </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>99</v>
       </c>
@@ -2502,10 +2486,8 @@
       <c r="AU14" s="3">
         <v>1</v>
       </c>
-      <c r="AV14" s="18"/>
-      <c r="AW14" s="18"/>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
@@ -2591,10 +2573,8 @@
       <c r="AU15" s="2">
         <v>1</v>
       </c>
-      <c r="AV15" s="18"/>
-      <c r="AW15" s="18"/>
-    </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>101</v>
       </c>
@@ -2688,10 +2668,8 @@
       <c r="AU16" s="2">
         <v>1</v>
       </c>
-      <c r="AV16" s="18"/>
-      <c r="AW16" s="18"/>
-    </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>102</v>
       </c>
@@ -2779,10 +2757,8 @@
       <c r="AU17" s="2">
         <v>1</v>
       </c>
-      <c r="AV17" s="18"/>
-      <c r="AW17" s="18"/>
-    </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -2860,10 +2836,8 @@
       <c r="AU18" s="2">
         <v>1</v>
       </c>
-      <c r="AV18" s="18"/>
-      <c r="AW18" s="18"/>
-    </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>104</v>
       </c>
@@ -2935,10 +2909,8 @@
       <c r="AU19" s="11">
         <v>1</v>
       </c>
-      <c r="AV19" s="18"/>
-      <c r="AW19" s="18"/>
-    </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>105</v>
       </c>
@@ -3034,10 +3006,8 @@
       <c r="AU20" s="2">
         <v>1</v>
       </c>
-      <c r="AV20" s="18"/>
-      <c r="AW20" s="18"/>
-    </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>106</v>
       </c>
@@ -3133,10 +3103,8 @@
       <c r="AU21" s="2">
         <v>1</v>
       </c>
-      <c r="AV21" s="18"/>
-      <c r="AW21" s="18"/>
-    </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>109</v>
       </c>
@@ -3232,10 +3200,8 @@
       <c r="AU22" s="2">
         <v>1</v>
       </c>
-      <c r="AV22" s="18"/>
-      <c r="AW22" s="18"/>
-    </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>110</v>
       </c>
@@ -3331,10 +3297,8 @@
       <c r="AU23" s="2">
         <v>1</v>
       </c>
-      <c r="AV23" s="18"/>
-      <c r="AW23" s="18"/>
-    </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>111</v>
       </c>
@@ -3430,10 +3394,8 @@
       <c r="AU24" s="2">
         <v>1</v>
       </c>
-      <c r="AV24" s="18"/>
-      <c r="AW24" s="18"/>
-    </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>114</v>
       </c>
@@ -3529,10 +3491,8 @@
       <c r="AU25" s="2">
         <v>1</v>
       </c>
-      <c r="AV25" s="18"/>
-      <c r="AW25" s="18"/>
-    </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>113</v>
       </c>
@@ -3628,10 +3588,8 @@
       <c r="AU26" s="2">
         <v>1</v>
       </c>
-      <c r="AV26" s="18"/>
-      <c r="AW26" s="18"/>
-    </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>112</v>
       </c>
@@ -3727,10 +3685,8 @@
       <c r="AU27" s="2">
         <v>1</v>
       </c>
-      <c r="AV27" s="18"/>
-      <c r="AW27" s="18"/>
-    </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -3810,10 +3766,8 @@
       <c r="AU28" s="3">
         <v>1</v>
       </c>
-      <c r="AV28" s="18"/>
-      <c r="AW28" s="18"/>
-    </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>116</v>
       </c>
@@ -3899,10 +3853,8 @@
       <c r="AU29" s="2">
         <v>1</v>
       </c>
-      <c r="AV29" s="18"/>
-      <c r="AW29" s="18"/>
-    </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>117</v>
       </c>
@@ -3996,10 +3948,8 @@
       <c r="AU30" s="2">
         <v>1</v>
       </c>
-      <c r="AV30" s="18"/>
-      <c r="AW30" s="18"/>
-    </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>118</v>
       </c>
@@ -4087,10 +4037,8 @@
       <c r="AU31" s="2">
         <v>1</v>
       </c>
-      <c r="AV31" s="18"/>
-      <c r="AW31" s="18"/>
-    </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>119</v>
       </c>
@@ -4168,10 +4116,8 @@
       <c r="AU32" s="2">
         <v>1</v>
       </c>
-      <c r="AV32" s="18"/>
-      <c r="AW32" s="18"/>
-    </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>120</v>
       </c>
@@ -4243,10 +4189,8 @@
       <c r="AU33" s="11">
         <v>1</v>
       </c>
-      <c r="AV33" s="18"/>
-      <c r="AW33" s="18"/>
-    </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>121</v>
       </c>
@@ -4342,10 +4286,8 @@
       <c r="AU34" s="2">
         <v>1</v>
       </c>
-      <c r="AV34" s="18"/>
-      <c r="AW34" s="18"/>
-    </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>122</v>
       </c>
@@ -4441,8 +4383,6 @@
       <c r="AU35" s="2">
         <v>1</v>
       </c>
-      <c r="AV35" s="18"/>
-      <c r="AW35" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>